<commit_message>
þurfti að breyta einni lýsingu í 2.xlsx/áætlun
git-svn-id: https://tgapc93.rhi.hi.is/svn/softdev/2013/hopur19@8246 5d233661-44a1-474e-bded-f455fa16cf90
</commit_message>
<xml_diff>
--- a/2.xlsx
+++ b/2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="25580" windowHeight="15540" tabRatio="658" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="658" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Verkáætlun" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="81">
   <si>
     <t>Ítrun 1</t>
   </si>
@@ -201,12 +201,6 @@
     <t>Hanna útlit</t>
   </si>
   <si>
-    <t>Forrit sem varar einstakling við ef verð fellur innan marka sem hann hefur sett</t>
-  </si>
-  <si>
-    <t>Forrit sem bendir einstakling á ef fyrirtæki gengur vel</t>
-  </si>
-  <si>
     <t>Verkþættir ítrunar 1</t>
   </si>
   <si>
@@ -267,7 +261,10 @@
     <t>Setja upp unittest prófanir fyrir það sem gert er í ítrun þrjú.</t>
   </si>
   <si>
-    <t>Hægt á að vera að stilla forritið þannig að það gefi frá sér aðvörun þegar stærð fer út fyrir ákveðinn ramma og bendir á ef fyrirtæki virðist vera ganga vel.</t>
+    <t>Forritið þarf að geta sagt hvort eigi að kaupa eða selja.</t>
+  </si>
+  <si>
+    <t>Forritið bendir notanda á hvort vissara sé að kaupa eða selja</t>
   </si>
 </sst>
 </file>
@@ -805,7 +802,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -819,8 +816,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1061,6 +1060,12 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1070,26 +1075,37 @@
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1422,7 +1438,7 @@
   <dimension ref="A2:AA37"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="R31" sqref="R31"/>
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1551,21 +1567,21 @@
         <v>7</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E5" s="33"/>
       <c r="F5" s="33" t="s">
         <v>7</v>
       </c>
       <c r="G5" s="33" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H5" s="33"/>
       <c r="I5" s="33" t="s">
         <v>7</v>
       </c>
       <c r="J5" s="33" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K5" s="38"/>
       <c r="M5" s="33"/>
@@ -1574,14 +1590,14 @@
         <v>7</v>
       </c>
       <c r="P5" s="33" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Q5" s="33"/>
       <c r="R5" s="33" t="s">
         <v>7</v>
       </c>
       <c r="S5" s="33" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="T5" s="38"/>
       <c r="U5" s="1"/>
@@ -1743,7 +1759,7 @@
       </c>
       <c r="X9" s="1"/>
       <c r="Y9" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Z9" s="2">
         <f>(4*2)*0.8</f>
@@ -1813,7 +1829,7 @@
         <v>1</v>
       </c>
       <c r="J12" s="33" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K12" s="38"/>
       <c r="L12" s="33"/>
@@ -1831,21 +1847,21 @@
         <v>7</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E13" s="33"/>
       <c r="F13" s="33" t="s">
         <v>7</v>
       </c>
       <c r="G13" s="33" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H13" s="33"/>
       <c r="I13" s="33" t="s">
         <v>7</v>
       </c>
       <c r="J13" s="33" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K13" s="38"/>
       <c r="L13" s="33"/>
@@ -1986,7 +2002,7 @@
       </c>
       <c r="X17" s="1"/>
       <c r="Y17" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Z17" s="2">
         <f>(4*2.5)*0.7</f>
@@ -2077,7 +2093,7 @@
         <v>1</v>
       </c>
       <c r="S20" s="33" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="T20" s="38"/>
     </row>
@@ -2088,21 +2104,21 @@
         <v>7</v>
       </c>
       <c r="D21" s="33" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E21" s="33"/>
       <c r="F21" s="33" t="s">
         <v>7</v>
       </c>
       <c r="G21" s="33" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H21" s="33"/>
       <c r="I21" s="33" t="s">
         <v>7</v>
       </c>
       <c r="J21" s="33" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K21" s="38"/>
       <c r="M21" s="33"/>
@@ -2110,15 +2126,15 @@
       <c r="O21" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="P21" s="33" t="s">
-        <v>81</v>
+      <c r="P21" s="85" t="s">
+        <v>79</v>
       </c>
       <c r="Q21" s="33"/>
       <c r="R21" s="33" t="s">
         <v>7</v>
       </c>
       <c r="S21" s="33" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="T21" s="38"/>
     </row>
@@ -2269,11 +2285,11 @@
         <v>14</v>
       </c>
       <c r="W25" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="X25" s="1"/>
       <c r="Y25" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Z25" s="2">
         <f>(4*3.75)*0.8</f>
@@ -2339,7 +2355,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="12.75" customHeight="1">
       <c r="D1" s="76" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1">
@@ -3210,10 +3226,10 @@
     </row>
     <row r="54" spans="1:12" ht="12.75" customHeight="1">
       <c r="B54" s="20"/>
-      <c r="C54" s="83" t="s">
+      <c r="C54" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="D54" s="84"/>
+      <c r="D54" s="81"/>
       <c r="E54" s="30"/>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
@@ -3268,16 +3284,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:G18"/>
     <mergeCell ref="I18:J18"/>
     <mergeCell ref="C54:D54"/>
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="F28:G28"/>
     <mergeCell ref="C44:D44"/>
     <mergeCell ref="F44:G44"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:G18"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3316,7 +3332,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="12.75" customHeight="1">
       <c r="D1" s="77" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1">
@@ -3416,20 +3432,20 @@
     <row r="8" spans="1:12" ht="12.75" customHeight="1">
       <c r="A8" s="53"/>
       <c r="B8" s="69"/>
-      <c r="C8" s="80" t="s">
+      <c r="C8" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="81"/>
+      <c r="D8" s="83"/>
       <c r="E8" s="69"/>
-      <c r="F8" s="80" t="s">
+      <c r="F8" s="82" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="81"/>
+      <c r="G8" s="83"/>
       <c r="H8" s="69"/>
-      <c r="I8" s="80" t="s">
+      <c r="I8" s="82" t="s">
         <v>33</v>
       </c>
-      <c r="J8" s="81"/>
+      <c r="J8" s="83"/>
       <c r="K8" s="69"/>
       <c r="L8" s="54"/>
     </row>
@@ -3596,20 +3612,20 @@
     <row r="18" spans="1:12" ht="12.75" customHeight="1">
       <c r="A18" s="53"/>
       <c r="B18" s="69"/>
-      <c r="C18" s="80" t="s">
+      <c r="C18" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="81"/>
+      <c r="D18" s="83"/>
       <c r="E18" s="69"/>
-      <c r="F18" s="80" t="s">
+      <c r="F18" s="82" t="s">
         <v>29</v>
       </c>
-      <c r="G18" s="81"/>
+      <c r="G18" s="83"/>
       <c r="H18" s="69"/>
-      <c r="I18" s="80" t="s">
+      <c r="I18" s="82" t="s">
         <v>33</v>
       </c>
-      <c r="J18" s="81"/>
+      <c r="J18" s="83"/>
       <c r="K18" s="69"/>
       <c r="L18" s="54"/>
     </row>
@@ -3712,7 +3728,7 @@
         <v>1</v>
       </c>
       <c r="D24" s="56" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E24" s="70"/>
       <c r="F24" s="71"/>
@@ -3776,18 +3792,18 @@
     <row r="28" spans="1:12" ht="12.75" customHeight="1">
       <c r="A28" s="53"/>
       <c r="B28" s="69"/>
-      <c r="C28" s="80" t="s">
+      <c r="C28" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="81"/>
+      <c r="D28" s="83"/>
       <c r="E28" s="69"/>
-      <c r="F28" s="80" t="s">
+      <c r="F28" s="82" t="s">
         <v>29</v>
       </c>
-      <c r="G28" s="81"/>
+      <c r="G28" s="83"/>
       <c r="H28" s="70"/>
-      <c r="I28" s="82"/>
-      <c r="J28" s="82"/>
+      <c r="I28" s="84"/>
+      <c r="J28" s="84"/>
       <c r="K28" s="72"/>
       <c r="L28" s="54"/>
     </row>
@@ -4168,8 +4184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -4186,7 +4202,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="12.75" customHeight="1">
       <c r="D1" s="76" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="12.75" customHeight="1">
@@ -4420,7 +4436,7 @@
       <c r="H18" s="20"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" ht="12.75" customHeight="1">
+    <row r="19" spans="1:9" ht="37" customHeight="1">
       <c r="A19" s="5"/>
       <c r="B19" s="20"/>
       <c r="C19" s="16" t="s">
@@ -4743,8 +4759,8 @@
       <c r="C43" s="17"/>
       <c r="D43" s="17"/>
       <c r="E43" s="4"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
+      <c r="F43" s="88"/>
+      <c r="G43" s="88"/>
       <c r="H43" s="25"/>
     </row>
     <row r="44" spans="1:9" ht="12.75" customHeight="1">
@@ -4753,29 +4769,23 @@
         <v>28</v>
       </c>
       <c r="D44" s="79"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="78" t="s">
-        <v>29</v>
-      </c>
-      <c r="G44" s="79"/>
-      <c r="H44" s="20"/>
-    </row>
-    <row r="45" spans="1:9" ht="12.75" customHeight="1">
+      <c r="E44" s="86"/>
+      <c r="F44" s="89"/>
+      <c r="G44" s="89"/>
+      <c r="H44" s="87"/>
+    </row>
+    <row r="45" spans="1:9" ht="36" customHeight="1">
       <c r="B45" s="20"/>
       <c r="C45" s="16" t="s">
         <v>7</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E45" s="20"/>
-      <c r="F45" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="G45" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="H45" s="20"/>
+        <v>80</v>
+      </c>
+      <c r="E45" s="86"/>
+      <c r="F45" s="89"/>
+      <c r="G45" s="89"/>
+      <c r="H45" s="87"/>
     </row>
     <row r="46" spans="1:9" ht="12.75" customHeight="1">
       <c r="B46" s="20"/>
@@ -4785,22 +4795,18 @@
       <c r="D46" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E46" s="20"/>
-      <c r="F46" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="G46" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H46" s="20"/>
+      <c r="E46" s="86"/>
+      <c r="F46" s="89"/>
+      <c r="G46" s="89"/>
+      <c r="H46" s="87"/>
     </row>
     <row r="47" spans="1:9" ht="12.75" customHeight="1">
       <c r="B47" s="28"/>
       <c r="C47" s="17"/>
       <c r="D47" s="17"/>
       <c r="E47" s="14"/>
-      <c r="F47" s="17"/>
-      <c r="G47" s="17"/>
+      <c r="F47" s="46"/>
+      <c r="G47" s="46"/>
       <c r="H47" s="13"/>
     </row>
     <row r="48" spans="1:9" ht="12.75" customHeight="1">
@@ -4832,7 +4838,7 @@
         <v>1</v>
       </c>
       <c r="D50" s="56" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E50" s="70"/>
       <c r="F50" s="4"/>
@@ -4879,10 +4885,10 @@
     </row>
     <row r="54" spans="1:9" ht="12.75" customHeight="1">
       <c r="B54" s="69"/>
-      <c r="C54" s="80" t="s">
+      <c r="C54" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="D54" s="81"/>
+      <c r="D54" s="83"/>
       <c r="E54" s="69"/>
       <c r="F54" s="78" t="s">
         <v>29</v>
@@ -4890,7 +4896,7 @@
       <c r="G54" s="79"/>
       <c r="H54" s="20"/>
     </row>
-    <row r="55" spans="1:9" ht="12.75" customHeight="1">
+    <row r="55" spans="1:9" ht="24" customHeight="1">
       <c r="B55" s="69"/>
       <c r="C55" s="61" t="s">
         <v>7</v>
@@ -4934,11 +4940,10 @@
       <c r="H57" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="9">
     <mergeCell ref="F54:G54"/>
     <mergeCell ref="C54:D54"/>
     <mergeCell ref="C44:D44"/>
-    <mergeCell ref="F44:G44"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="C18:D18"/>

</xml_diff>